<commit_message>
Add jquery, replace data object with cdn data
</commit_message>
<xml_diff>
--- a/docs/ЦТВ Новгородской области_12-12-2018_03-58-06.xlsx
+++ b/docs/ЦТВ Новгородской области_12-12-2018_03-58-06.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/WorkProjects/NovOblMap/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B6090-B0D0-9E45-8896-DC03FC945243}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EF3A9F-97E2-2C4C-8949-63137E3370A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ЦТВ Новгородской области" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
   <si>
     <t>58.52281</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>сeh</t>
+  </si>
+  <si>
+    <t>сh1mux</t>
+  </si>
+  <si>
+    <t>сh2mux</t>
   </si>
 </sst>
 </file>
@@ -396,6 +405,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D93C981-E7DA-AD47-9F44-EC652E789C5B}" name="Таблица2" displayName="Таблица2" ref="A1:F36" totalsRowShown="0">
+  <autoFilter ref="A1:F36" xr:uid="{86B67A07-ACA9-BC4C-A22C-83A0C5794221}"/>
+  <sortState ref="A2:F36">
+    <sortCondition ref="B1:B36"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{57FACEB2-BAB2-1B4A-9022-AD69D2853010}" name="сeh"/>
+    <tableColumn id="2" xr3:uid="{FEAE71C1-3BC0-F24A-BAB7-5CC774D5BE2C}" name="name"/>
+    <tableColumn id="3" xr3:uid="{088B3637-2AAE-A54B-ACC5-6BB1261C6C8B}" name="lat"/>
+    <tableColumn id="4" xr3:uid="{A67B88D4-FEB1-B34F-8B20-A9EECD440847}" name="len"/>
+    <tableColumn id="5" xr3:uid="{C5582314-7618-A444-959D-3A27EA27103A}" name="сh1mux"/>
+    <tableColumn id="6" xr3:uid="{A58CCD98-27F6-024B-88D6-0EDC4D57EF75}" name="сh2mux"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -720,417 +747,747 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="3" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>26</v>
+      </c>
+      <c r="F2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>51</v>
+      </c>
+      <c r="F6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8">
+        <v>26</v>
+      </c>
+      <c r="F8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11">
+        <v>51</v>
+      </c>
+      <c r="F11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>51</v>
+      </c>
+      <c r="F12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>51</v>
+      </c>
+      <c r="F13">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14">
+        <v>51</v>
+      </c>
+      <c r="F14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>26</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>51</v>
+      </c>
+      <c r="F16">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <v>51</v>
+      </c>
+      <c r="F17">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>26</v>
+      </c>
+      <c r="F18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F19">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>51</v>
+      </c>
+      <c r="F21">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22">
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23">
+        <v>51</v>
+      </c>
+      <c r="F23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="F24">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25">
+        <v>40</v>
+      </c>
+      <c r="F25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26">
+        <v>51</v>
+      </c>
+      <c r="F26">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27">
+        <v>51</v>
+      </c>
+      <c r="F27">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>51</v>
+      </c>
+      <c r="F30">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33">
+        <v>26</v>
+      </c>
+      <c r="F33">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34">
+        <v>26</v>
+      </c>
+      <c r="F34">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35">
+        <v>23</v>
+      </c>
+      <c r="F35">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="F36">
         <v>57</v>
       </c>
-      <c r="C34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>86</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C37">
-    <sortCondition ref="C37"/>
+  <sortState ref="A2:B37">
+    <sortCondition ref="B37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add lines from main cehs to their slave units
</commit_message>
<xml_diff>
--- a/docs/ЦТВ Новгородской области_12-12-2018_03-58-06.xlsx
+++ b/docs/ЦТВ Новгородской области_12-12-2018_03-58-06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/WorkProjects/NovOblMap/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EF3A9F-97E2-2C4C-8949-63137E3370A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712DDB55-55D3-CB4B-9FDB-1155882C47A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,13 +346,13 @@
     <t>name</t>
   </si>
   <si>
-    <t>сeh</t>
-  </si>
-  <si>
     <t>сh1mux</t>
   </si>
   <si>
     <t>сh2mux</t>
+  </si>
+  <si>
+    <t>ceh</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
     <sortCondition ref="B1:B36"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{57FACEB2-BAB2-1B4A-9022-AD69D2853010}" name="сeh"/>
+    <tableColumn id="1" xr3:uid="{57FACEB2-BAB2-1B4A-9022-AD69D2853010}" name="ceh"/>
     <tableColumn id="2" xr3:uid="{FEAE71C1-3BC0-F24A-BAB7-5CC774D5BE2C}" name="name"/>
     <tableColumn id="3" xr3:uid="{088B3637-2AAE-A54B-ACC5-6BB1261C6C8B}" name="lat"/>
     <tableColumn id="4" xr3:uid="{A67B88D4-FEB1-B34F-8B20-A9EECD440847}" name="len"/>
@@ -749,9 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -763,7 +761,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>107</v>
@@ -775,10 +773,10 @@
         <v>106</v>
       </c>
       <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
         <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add webpack bundler, separate routes and data to files
</commit_message>
<xml_diff>
--- a/docs/ЦТВ Новгородской области_12-12-2018_03-58-06.xlsx
+++ b/docs/ЦТВ Новгородской области_12-12-2018_03-58-06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/WorkProjects/NovOblMap/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712DDB55-55D3-CB4B-9FDB-1155882C47A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2817FE41-9F1C-0E4B-93A9-B1C513C16C6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,7 +749,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>